<commit_message>
Fixed iteration to next story through XPATH
</commit_message>
<xml_diff>
--- a/robot_Anton_Roscher/news_searches.xlsx
+++ b/robot_Anton_Roscher/news_searches.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="garmin" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="garmin1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="garmin2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1125,4 +1127,768 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Story_Content</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Date_Created</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Image_Filename</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Garmin Ltd</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Japan’s Nikkei 225 share benchmark has touched an all-time high, bypassing its previous record set in December 1989.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2024-02-22 03:57:37</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Garmin_Ltd.png.png</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Story_Content</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Date_Created</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Image_Filename</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Palo Alto Networks, Keysight fall; Garmin, Toll Brothers rise, Wednesday, 2/21/2024</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Stocks that traded heavily or had substantial price changes on Wednesday: Palo Alto Networks, Keysight fall; Garmin, Toll Brothers rise.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-02-21 21:24:35</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Palo_Alto_Networks_Keysight_fall;_Garmin_Toll_Brothers_rise_Wednesday_2/21/2024.png.png</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated save image function using RPA selenium method
</commit_message>
<xml_diff>
--- a/robot_Anton_Roscher/news_searches.xlsx
+++ b/robot_Anton_Roscher/news_searches.xlsx
@@ -19,6 +19,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trump5" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trump6" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trump7" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trump8" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2547,7 +2548,6 @@
           <t>One Notable Number</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
           <t>2024-04-19 08:46:52</t>
@@ -3097,6 +3097,85 @@
       </c>
       <c r="F31" t="b">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Story_Content</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Date_Created</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Image_Filename</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>word_count</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>title_has_money</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Pennsylvania board’s cancellation of gay actor’s school visit ill-advised, education leaders say</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>The superintendent and several other top officials of a Pennsylvania school district say their school board’s cancellation of a gay actor’s visit to a middle school was premature and ill-advised.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-04-19 15:23:55</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Pennsylvania_board’s_cancellation_of_gay_actor’s_school_visit_ill-advised_education_leaders_say.png.png</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>42</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>